<commit_message>
AGD merged to the JGA excel
</commit_message>
<xml_diff>
--- a/JGA_metadata.xlsx
+++ b/JGA_metadata.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="809">
   <si>
     <t>E-mail</t>
     <phoneticPr fontId="1"/>
@@ -1292,13 +1292,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t># それぞれのエクセルシートが JGA メタデータオブジェクトに対応しています。</t>
-    <rPh sb="32" eb="34">
-      <t>タイオウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>JGA へのデータ登録については、以下のウェブサイトをご覧ください。</t>
     <rPh sb="9" eb="11">
       <t>トウロク</t>
@@ -1312,13 +1305,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>連絡先: jga@ddbj.nig.ac.jp</t>
-    <rPh sb="0" eb="3">
-      <t>レンラクサキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>必須項目</t>
     <rPh sb="0" eb="2">
       <t>ヒッス</t>
@@ -1466,19 +1452,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t># 登録日。JGA で記入します</t>
-    <rPh sb="2" eb="4">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ビ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>キニュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Submission Date</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1488,32 +1461,6 @@
   </si>
   <si>
     <t>Reverse</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>JGA メタデータ登録シート</t>
-    <rPh sb="9" eb="11">
-      <t>トウロク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>JGA へデータを登録するためには、データ提供を NBDC に申請し承認されている必要があります。</t>
-    <rPh sb="9" eb="11">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>シンセイ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ショウニン</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ヒツヨウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2297,25 +2244,6 @@
     <t># Analysis の概要</t>
     <rPh sb="12" eb="14">
       <t>ガイヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t># データ提供申請に対し NBDC から発行された Research ID (例: hum0004)</t>
-    <rPh sb="5" eb="7">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>シンセイ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ハッコウ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>レイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3807,71 +3735,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <t># "Hold" か "Release immediately" を選択。"Hold" の場合、データの共有が可能になったら JGA チームに連絡します。公開予定日を指定することはできません。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>データは submission (JSUB) 単位で公開されます。公開予定時期が異なるデータは submission を分けてください。</t>
-    </r>
-    <rPh sb="34" eb="36">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>キョウユウ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>カノウ</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>レンラク</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>コウカイ</t>
-    </rPh>
-    <rPh sb="79" eb="82">
-      <t>ヨテイビ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="119" eb="121">
-      <t>タンイ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>コウカイ</t>
-    </rPh>
-    <rPh sb="129" eb="131">
-      <t>コウカイ</t>
-    </rPh>
-    <rPh sb="131" eb="133">
-      <t>ヨテイ</t>
-    </rPh>
-    <rPh sb="133" eb="135">
-      <t>ジキ</t>
-    </rPh>
-    <rPh sb="136" eb="137">
-      <t>コト</t>
-    </rPh>
-    <rPh sb="156" eb="157">
-      <t>ワ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>データは submission (JSUB) 単位で公開されます。公開予定時期が異なるデータは submission を分けてください。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>NBDC Number (hum)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4235,6 +4098,166 @@
     </rPh>
     <rPh sb="42" eb="44">
       <t>キサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JGA/AGD メタデータ登録シート</t>
+    <rPh sb="13" eb="15">
+      <t>トウロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JGA/AGD へデータを登録するためには、データ提供を NBDC に申請し承認されている必要があります。</t>
+    <rPh sb="13" eb="15">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>シンセイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ショウニン</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>データは submission (JSUB/ASUB) 単位で公開されます。公開予定時期が異なるデータは submission を分けてください。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AGD へのデータ登録については、以下のウェブサイトをご覧ください。</t>
+    <rPh sb="9" eb="11">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ラン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://www.ddbj.nig.ac.jp/agd/index.html</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AGD 統合</t>
+    <rPh sb="4" eb="6">
+      <t>トウゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># データ提供申請に対し NBDC から発行された Research ID (例: hum0004)。AGD の場合、agd0000 形式の ID (例: agd0001)</t>
+    <rPh sb="5" eb="7">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シンセイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ハッコウ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>レイ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>ケイシキ</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t># "Hold" か "Release immediately" を選択。"Hold" の場合、データの共有が可能になったら JGA/AGD チームに連絡します。公開予定日を指定することはできません。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>データは submission (JSUB/ASUB) 単位で公開されます。公開予定時期が異なるデータは submission を分けてください。</t>
+    </r>
+    <rPh sb="34" eb="36">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>キョウユウ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>レンラク</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>コウカイ</t>
+    </rPh>
+    <rPh sb="83" eb="86">
+      <t>ヨテイビ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="128" eb="130">
+      <t>タンイ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>コウカイ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>コウカイ</t>
+    </rPh>
+    <rPh sb="140" eb="142">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="142" eb="144">
+      <t>ジキ</t>
+    </rPh>
+    <rPh sb="145" eb="146">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="165" eb="166">
+      <t>ワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># 登録日</t>
+    <rPh sb="2" eb="4">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ビ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># それぞれのエクセルシートが JGA/AGD メタデータオブジェクトに対応しています。</t>
+    <rPh sb="36" eb="38">
+      <t>タイオウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4779,7 +4802,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4790,215 +4813,232 @@
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" s="8" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" s="8" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" s="22" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A7" s="8"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A11" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A9" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A12" s="3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A14" s="1" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A15" s="3" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A17" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A18" s="23"/>
+      <c r="B18" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A12" s="3" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A13" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A15" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A19" s="24"/>
+      <c r="B19" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A20" s="25"/>
+      <c r="B20" s="1" t="s">
         <v>404</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A16" s="23"/>
-      <c r="B16" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A17" s="24"/>
-      <c r="B17" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A18" s="25"/>
-      <c r="B18" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A21" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A24" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A24" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A25" s="9">
-        <v>44678</v>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A26" s="1" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A27" s="1" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A28" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="B28" s="9">
-        <v>42285</v>
+      <c r="A27" s="9">
+        <v>44918</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="B29" s="9">
-        <v>42429</v>
+        <v>579</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>599</v>
+        <v>580</v>
       </c>
       <c r="B30" s="9">
-        <v>42430</v>
+        <v>42285</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>650</v>
+        <v>590</v>
       </c>
       <c r="B31" s="9">
-        <v>42486</v>
+        <v>42429</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>655</v>
+        <v>593</v>
       </c>
       <c r="B32" s="9">
-        <v>42760</v>
+        <v>42430</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>692</v>
+        <v>644</v>
       </c>
       <c r="B33" s="9">
-        <v>42935</v>
+        <v>42486</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>726</v>
+        <v>649</v>
       </c>
       <c r="B34" s="9">
-        <v>42935</v>
+        <v>42760</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>741</v>
+        <v>686</v>
       </c>
       <c r="B35" s="9">
-        <v>43227</v>
+        <v>42935</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>749</v>
+        <v>720</v>
       </c>
       <c r="B36" s="9">
-        <v>44103</v>
+        <v>42935</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>759</v>
+        <v>735</v>
       </c>
       <c r="B37" s="9">
-        <v>44622</v>
+        <v>43227</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
-        <v>791</v>
+        <v>743</v>
       </c>
       <c r="B38" s="9">
+        <v>44103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A39" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B39" s="9">
+        <v>44622</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A40" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B40" s="9">
         <v>44678</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A41" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B41" s="9">
+        <v>44918</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
     <hyperlink ref="A12" r:id="rId1"/>
+    <hyperlink ref="A15" r:id="rId2" display="https://www.ddbj.nig.ac.jp/jga/index.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5063,7 +5103,7 @@
         <v>361</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="K1" s="30" t="s">
         <v>334</v>
@@ -5075,13 +5115,13 @@
         <v>334</v>
       </c>
       <c r="N1" s="30" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="O1" s="30" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="P1" s="30" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="Q1" s="4"/>
     </row>
@@ -5105,13 +5145,13 @@
         <v>362</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>336</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>329</v>
@@ -5123,13 +5163,13 @@
         <v>327</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="P2" s="1" t="b">
         <v>1</v>
@@ -5155,7 +5195,7 @@
         <v>363</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>335</v>
@@ -5164,22 +5204,22 @@
         <v>355</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.5">
@@ -5205,16 +5245,16 @@
         <v>356</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.5">
@@ -5234,22 +5274,22 @@
         <v>303</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>357</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>335</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.5">
@@ -5266,7 +5306,7 @@
         <v>282</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>358</v>
@@ -5281,7 +5321,7 @@
         <v>370</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.5">
@@ -5304,7 +5344,7 @@
         <v>359</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>378</v>
@@ -5313,7 +5353,7 @@
         <v>371</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.5">
@@ -5336,7 +5376,7 @@
         <v>360</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>379</v>
@@ -5345,7 +5385,7 @@
         <v>372</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.5">
@@ -5362,10 +5402,10 @@
         <v>306</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>339</v>
@@ -5374,7 +5414,7 @@
         <v>373</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.5">
@@ -5388,22 +5428,22 @@
         <v>286</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.5">
@@ -5420,19 +5460,19 @@
         <v>307</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>328</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.5">
@@ -5440,28 +5480,28 @@
         <v>237</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>308</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.5">
@@ -5472,16 +5512,16 @@
         <v>254</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>309</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>340</v>
@@ -5490,7 +5530,7 @@
         <v>374</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.5">
@@ -5501,13 +5541,13 @@
         <v>253</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>310</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>242</v>
@@ -5519,7 +5559,7 @@
         <v>375</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.5">
@@ -5527,25 +5567,25 @@
         <v>240</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>311</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.5">
@@ -5553,10 +5593,10 @@
         <v>241</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>312</v>
@@ -5565,10 +5605,10 @@
         <v>380</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.5">
@@ -5585,15 +5625,15 @@
         <v>313</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B18" s="1" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>289</v>
@@ -5602,10 +5642,10 @@
         <v>314</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.5">
@@ -5613,21 +5653,21 @@
         <v>257</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>315</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="N19" s="17" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B20" s="1" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>290</v>
@@ -5636,49 +5676,49 @@
         <v>316</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="N20" s="17" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B21" s="1" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>291</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="N21" s="17" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B22" s="1" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>381</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B23" s="1" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>292</v>
@@ -5690,12 +5730,12 @@
         <v>382</v>
       </c>
       <c r="N23" s="17" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B24" s="1" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>293</v>
@@ -5707,12 +5747,12 @@
         <v>383</v>
       </c>
       <c r="N24" s="17" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B25" s="1" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>294</v>
@@ -5724,12 +5764,12 @@
         <v>384</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B26" s="1" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>295</v>
@@ -5738,15 +5778,15 @@
         <v>320</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="N26" s="17" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B27" s="1" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>296</v>
@@ -5755,15 +5795,15 @@
         <v>321</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="N27" s="17" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B28" s="1" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>297</v>
@@ -5772,18 +5812,18 @@
         <v>322</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B29" s="1" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>298</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>385</v>
@@ -5791,7 +5831,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B30" s="1" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>299</v>
@@ -5805,7 +5845,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B31" s="1" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>270</v>
@@ -5819,10 +5859,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B32" s="1" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>388</v>
@@ -5855,7 +5895,7 @@
         <v>260</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>391</v>
@@ -5866,7 +5906,7 @@
         <v>261</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>392</v>
@@ -5877,7 +5917,7 @@
         <v>262</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>393</v>
@@ -5912,7 +5952,7 @@
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B41" s="1" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>397</v>
@@ -5920,15 +5960,15 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B42" s="1" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B43" s="1" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>398</v>
@@ -5939,31 +5979,31 @@
         <v>266</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B45" s="1" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B46" s="1" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B47" s="1" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.5">
@@ -5971,31 +6011,31 @@
         <v>267</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B49" s="1" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B50" s="1" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B51" s="1" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.5">
@@ -6013,62 +6053,62 @@
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B54" s="1" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B55" s="1" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B56" s="1" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B57" s="1" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B58" s="1" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B59" s="1" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B60" s="1" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B61" s="1" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B62" s="1" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B63" s="1" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B64" s="1" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B65" s="1" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -6086,9 +6126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.6640625" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
@@ -6101,12 +6139,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>554</v>
+        <v>805</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="26" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
@@ -6114,12 +6152,12 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>754</v>
+        <v>806</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="26" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
@@ -6130,7 +6168,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
@@ -6138,39 +6176,39 @@
         <v>13</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="29" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -6221,12 +6259,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>421</v>
+        <v>807</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A23" s="26" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.5">
@@ -6271,7 +6309,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
@@ -6287,7 +6325,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.5">
@@ -6321,7 +6359,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.5">
@@ -6337,33 +6375,33 @@
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="26" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.5">
@@ -6390,18 +6428,18 @@
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" s="26" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -6412,7 +6450,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
@@ -6434,12 +6472,12 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" s="27" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
@@ -6447,21 +6485,21 @@
     </row>
     <row r="30" spans="1:5" s="4" customFormat="1" ht="52.2" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" s="28" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
@@ -6488,7 +6526,7 @@
     </row>
     <row r="36" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.5">
@@ -6499,7 +6537,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.5">
@@ -6527,7 +6565,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.5">
@@ -6572,7 +6610,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
@@ -6602,18 +6640,18 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" s="27" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.5">
@@ -6684,40 +6722,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
@@ -6725,13 +6763,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>1</v>
@@ -6740,22 +6778,22 @@
         <v>353</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
@@ -7422,40 +7460,40 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="L1" s="33" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
@@ -7474,7 +7512,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>217</v>
@@ -7495,25 +7533,25 @@
         <v>222</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="L2" s="26" t="s">
+        <v>411</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>565</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="O2" s="26" t="s">
         <v>413</v>
       </c>
-      <c r="M2" s="27" t="s">
-        <v>571</v>
-      </c>
-      <c r="N2" s="26" t="s">
+      <c r="P2" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="O2" s="26" t="s">
-        <v>415</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>416</v>
-      </c>
       <c r="Q2" s="26" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.5">
@@ -7521,7 +7559,7 @@
         <v>116</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O3" s="1">
         <v>1</v>
@@ -7532,7 +7570,7 @@
         <v>117</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O4" s="1">
         <v>1</v>
@@ -7543,7 +7581,7 @@
         <v>118</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O5" s="1">
         <v>1</v>
@@ -7554,7 +7592,7 @@
         <v>119</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O6" s="1">
         <v>1</v>
@@ -7565,7 +7603,7 @@
         <v>120</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O7" s="1">
         <v>1</v>
@@ -7576,7 +7614,7 @@
         <v>121</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O8" s="1">
         <v>1</v>
@@ -7587,7 +7625,7 @@
         <v>122</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O9" s="1">
         <v>1</v>
@@ -7598,7 +7636,7 @@
         <v>123</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O10" s="1">
         <v>1</v>
@@ -7609,7 +7647,7 @@
         <v>124</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O11" s="1">
         <v>1</v>
@@ -7620,7 +7658,7 @@
         <v>125</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O12" s="1">
         <v>1</v>
@@ -7631,7 +7669,7 @@
         <v>126</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O13" s="1">
         <v>1</v>
@@ -7642,7 +7680,7 @@
         <v>127</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O14" s="1">
         <v>1</v>
@@ -7653,7 +7691,7 @@
         <v>128</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O15" s="1">
         <v>1</v>
@@ -7664,7 +7702,7 @@
         <v>129</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O16" s="1">
         <v>1</v>
@@ -7675,7 +7713,7 @@
         <v>130</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O17" s="1">
         <v>1</v>
@@ -7686,7 +7724,7 @@
         <v>131</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O18" s="1">
         <v>1</v>
@@ -7697,7 +7735,7 @@
         <v>132</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O19" s="1">
         <v>1</v>
@@ -7708,7 +7746,7 @@
         <v>133</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O20" s="1">
         <v>1</v>
@@ -7719,7 +7757,7 @@
         <v>134</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O21" s="1">
         <v>1</v>
@@ -7730,7 +7768,7 @@
         <v>135</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O22" s="1">
         <v>1</v>
@@ -7741,7 +7779,7 @@
         <v>136</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O23" s="1">
         <v>1</v>
@@ -7752,7 +7790,7 @@
         <v>137</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O24" s="1">
         <v>1</v>
@@ -7763,7 +7801,7 @@
         <v>138</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O25" s="1">
         <v>1</v>
@@ -7774,7 +7812,7 @@
         <v>139</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O26" s="1">
         <v>1</v>
@@ -7785,7 +7823,7 @@
         <v>140</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O27" s="1">
         <v>1</v>
@@ -7796,7 +7834,7 @@
         <v>141</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O28" s="1">
         <v>1</v>
@@ -7807,7 +7845,7 @@
         <v>142</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O29" s="1">
         <v>1</v>
@@ -7818,7 +7856,7 @@
         <v>143</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O30" s="1">
         <v>1</v>
@@ -7829,7 +7867,7 @@
         <v>144</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O31" s="1">
         <v>1</v>
@@ -7840,7 +7878,7 @@
         <v>145</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O32" s="1">
         <v>1</v>
@@ -7851,7 +7889,7 @@
         <v>146</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O33" s="1">
         <v>1</v>
@@ -7862,7 +7900,7 @@
         <v>147</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O34" s="1">
         <v>1</v>
@@ -7873,7 +7911,7 @@
         <v>148</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O35" s="1">
         <v>1</v>
@@ -7884,7 +7922,7 @@
         <v>149</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O36" s="1">
         <v>1</v>
@@ -7895,7 +7933,7 @@
         <v>150</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O37" s="1">
         <v>1</v>
@@ -7906,7 +7944,7 @@
         <v>151</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O38" s="1">
         <v>1</v>
@@ -7917,7 +7955,7 @@
         <v>152</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O39" s="1">
         <v>1</v>
@@ -7928,7 +7966,7 @@
         <v>153</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O40" s="1">
         <v>1</v>
@@ -7939,7 +7977,7 @@
         <v>154</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O41" s="1">
         <v>1</v>
@@ -7950,7 +7988,7 @@
         <v>155</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O42" s="1">
         <v>1</v>
@@ -7961,7 +7999,7 @@
         <v>156</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O43" s="1">
         <v>1</v>
@@ -7972,7 +8010,7 @@
         <v>157</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O44" s="1">
         <v>1</v>
@@ -7983,7 +8021,7 @@
         <v>158</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O45" s="1">
         <v>1</v>
@@ -7994,7 +8032,7 @@
         <v>159</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O46" s="1">
         <v>1</v>
@@ -8005,7 +8043,7 @@
         <v>160</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O47" s="1">
         <v>1</v>
@@ -8016,7 +8054,7 @@
         <v>161</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O48" s="1">
         <v>1</v>
@@ -8027,7 +8065,7 @@
         <v>162</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O49" s="1">
         <v>1</v>
@@ -8038,7 +8076,7 @@
         <v>163</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O50" s="1">
         <v>1</v>
@@ -8049,7 +8087,7 @@
         <v>164</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O51" s="1">
         <v>1</v>
@@ -8060,7 +8098,7 @@
         <v>165</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O52" s="1">
         <v>1</v>
@@ -8071,7 +8109,7 @@
         <v>166</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O53" s="1">
         <v>1</v>
@@ -8082,7 +8120,7 @@
         <v>167</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O54" s="1">
         <v>1</v>
@@ -8093,7 +8131,7 @@
         <v>168</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O55" s="1">
         <v>1</v>
@@ -8104,7 +8142,7 @@
         <v>169</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O56" s="1">
         <v>1</v>
@@ -8115,7 +8153,7 @@
         <v>170</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O57" s="1">
         <v>1</v>
@@ -8126,7 +8164,7 @@
         <v>171</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O58" s="1">
         <v>1</v>
@@ -8137,7 +8175,7 @@
         <v>172</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O59" s="1">
         <v>1</v>
@@ -8148,7 +8186,7 @@
         <v>173</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O60" s="1">
         <v>1</v>
@@ -8159,7 +8197,7 @@
         <v>174</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O61" s="1">
         <v>1</v>
@@ -8170,7 +8208,7 @@
         <v>175</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O62" s="1">
         <v>1</v>
@@ -8181,7 +8219,7 @@
         <v>176</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O63" s="1">
         <v>1</v>
@@ -8192,7 +8230,7 @@
         <v>177</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O64" s="1">
         <v>1</v>
@@ -8203,7 +8241,7 @@
         <v>178</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O65" s="1">
         <v>1</v>
@@ -8214,7 +8252,7 @@
         <v>179</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O66" s="1">
         <v>1</v>
@@ -8225,7 +8263,7 @@
         <v>180</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O67" s="1">
         <v>1</v>
@@ -8236,7 +8274,7 @@
         <v>181</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O68" s="1">
         <v>1</v>
@@ -8247,7 +8285,7 @@
         <v>182</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O69" s="1">
         <v>1</v>
@@ -8258,7 +8296,7 @@
         <v>183</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O70" s="1">
         <v>1</v>
@@ -8269,7 +8307,7 @@
         <v>184</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O71" s="1">
         <v>1</v>
@@ -8280,7 +8318,7 @@
         <v>185</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O72" s="1">
         <v>1</v>
@@ -8291,7 +8329,7 @@
         <v>186</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O73" s="1">
         <v>1</v>
@@ -8302,7 +8340,7 @@
         <v>187</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O74" s="1">
         <v>1</v>
@@ -8313,7 +8351,7 @@
         <v>188</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O75" s="1">
         <v>1</v>
@@ -8324,7 +8362,7 @@
         <v>189</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O76" s="1">
         <v>1</v>
@@ -8335,7 +8373,7 @@
         <v>190</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O77" s="1">
         <v>1</v>
@@ -8346,7 +8384,7 @@
         <v>191</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O78" s="1">
         <v>1</v>
@@ -8357,7 +8395,7 @@
         <v>192</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O79" s="1">
         <v>1</v>
@@ -8368,7 +8406,7 @@
         <v>193</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O80" s="1">
         <v>1</v>
@@ -8379,7 +8417,7 @@
         <v>194</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O81" s="1">
         <v>1</v>
@@ -8390,7 +8428,7 @@
         <v>195</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O82" s="1">
         <v>1</v>
@@ -8401,7 +8439,7 @@
         <v>196</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O83" s="1">
         <v>1</v>
@@ -8412,7 +8450,7 @@
         <v>197</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O84" s="1">
         <v>1</v>
@@ -8423,7 +8461,7 @@
         <v>198</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O85" s="1">
         <v>1</v>
@@ -8434,7 +8472,7 @@
         <v>199</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O86" s="1">
         <v>1</v>
@@ -8445,7 +8483,7 @@
         <v>200</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O87" s="1">
         <v>1</v>
@@ -8456,7 +8494,7 @@
         <v>201</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O88" s="1">
         <v>1</v>
@@ -8467,7 +8505,7 @@
         <v>202</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O89" s="1">
         <v>1</v>
@@ -8478,7 +8516,7 @@
         <v>203</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O90" s="1">
         <v>1</v>
@@ -8489,7 +8527,7 @@
         <v>204</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O91" s="1">
         <v>1</v>
@@ -8500,7 +8538,7 @@
         <v>205</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O92" s="1">
         <v>1</v>
@@ -8511,7 +8549,7 @@
         <v>206</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O93" s="1">
         <v>1</v>
@@ -8522,7 +8560,7 @@
         <v>207</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O94" s="1">
         <v>1</v>
@@ -8533,7 +8571,7 @@
         <v>208</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O95" s="1">
         <v>1</v>
@@ -8544,7 +8582,7 @@
         <v>209</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O96" s="1">
         <v>1</v>
@@ -8555,7 +8593,7 @@
         <v>210</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O97" s="1">
         <v>1</v>
@@ -8566,7 +8604,7 @@
         <v>211</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O98" s="1">
         <v>1</v>
@@ -8577,7 +8615,7 @@
         <v>212</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O99" s="1">
         <v>1</v>
@@ -8588,7 +8626,7 @@
         <v>213</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O100" s="1">
         <v>1</v>
@@ -8599,7 +8637,7 @@
         <v>214</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O101" s="1">
         <v>1</v>
@@ -8610,7 +8648,7 @@
         <v>215</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="O102" s="1">
         <v>1</v>
@@ -8702,22 +8740,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
@@ -8728,574 +8766,574 @@
         <v>331</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="30" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="30" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="30" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="30" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="30" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="30" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="30" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="30" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="30" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="30" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="30" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="30" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="30" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="30" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17" s="30" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18" s="30" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19" s="30" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21" s="30" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A22" s="30" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A23" s="30" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A24" s="30" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A25" s="30" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A26" s="30" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A27" s="30" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A28" s="30" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A29" s="30" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A30" s="30" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A31" s="30" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A32" s="30" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A33" s="30" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A34" s="30" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A35" s="30" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B35" s="4"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A36" s="30" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A37" s="30" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B37" s="4"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A38" s="30" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A39" s="30" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A40" s="30" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A41" s="30" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A42" s="30" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A43" s="30" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A44" s="30" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A45" s="30" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A46" s="30" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A47" s="30" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A48" s="30" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A49" s="30" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A50" s="30" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A51" s="30" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A52" s="30" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A53" s="30" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A54" s="30" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A55" s="30" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A56" s="30" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A57" s="30" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A58" s="30" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A59" s="30" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A60" s="30" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="B60" s="4"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A61" s="30" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A62" s="30" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A63" s="30" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A64" s="30" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A65" s="30" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A66" s="30" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A67" s="30" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A68" s="30" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A69" s="30" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A70" s="30" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A71" s="30" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A72" s="30" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A73" s="30" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A74" s="30" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A75" s="30" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A76" s="30" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A77" s="30" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A78" s="30" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A79" s="30" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A80" s="30" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A81" s="30" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A82" s="30" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A83" s="30" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A84" s="30" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A85" s="30" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A86" s="30" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A87" s="30" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A88" s="30" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A89" s="30" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A90" s="30" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A91" s="30" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A92" s="30" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A93" s="30" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A94" s="30" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A95" s="30" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A96" s="30" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A97" s="30" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A98" s="30" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A99" s="30" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A100" s="30" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A101" s="30" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A102" s="30" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -9336,65 +9374,65 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>553</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.5">
@@ -9402,13 +9440,13 @@
         <v>330</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>216</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>352</v>
@@ -9426,40 +9464,40 @@
         <v>333</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="Q2" s="31" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="R2" s="31" t="s">
+        <v>789</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>790</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>791</v>
+      </c>
+      <c r="U2" s="27" t="s">
         <v>797</v>
-      </c>
-      <c r="S2" s="31" t="s">
-        <v>798</v>
-      </c>
-      <c r="T2" s="31" t="s">
-        <v>799</v>
-      </c>
-      <c r="U2" s="27" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.5">
@@ -9467,7 +9505,7 @@
         <v>342</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.5">
@@ -9588,25 +9626,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
@@ -9614,7 +9652,7 @@
         <v>330</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>366</v>
@@ -9681,18 +9719,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" s="26" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change added sample attributes format
</commit_message>
<xml_diff>
--- a/JGA_metadata.xlsx
+++ b/JGA_metadata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B503AD2C-E82D-45F1-B0C5-28FCD16E1F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C1C74B-48DA-4FD8-88E8-CC5D1CE7E0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="813">
   <si>
     <t>E-mail</t>
     <phoneticPr fontId="1"/>
@@ -3419,72 +3419,6 @@
   </si>
   <si>
     <t>DOCUMENT</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t># Sample の表現型とサンプル属性を 名前:値; 名前:値; … の組み合わせで記載します。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>解析に必須な情報は必ず記載してください。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-例: age:37; smoke:yes; collection_date:2000-01-01</t>
-    </r>
-    <rPh sb="10" eb="13">
-      <t>ヒョウゲンケイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ゾクセイ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>アタイ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>ク</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>キサイ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>カイセキ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ヒッス</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>カナラ</t>
-    </rPh>
-    <rPh sb="60" eb="62">
-      <t>キサイ</t>
-    </rPh>
-    <rPh sb="70" eb="71">
-      <t>レイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4270,12 +4204,62 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Sample 追加属性の記載形式を変更</t>
+    <rPh sb="7" eb="11">
+      <t>ツイカゾクセイ</t>
+    </rPh>
+    <rPh sb="12" eb="16">
+      <t>キサイケイシキ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># L列以降に属性を追加して Sample を十分に記載してください。
+属性名 (例 age) を二行目に、対応する値 (例 40) を三行目以降に記載します。</t>
+    <rPh sb="7" eb="9">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジュウブン</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>キサイ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>レイ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>タイオウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>ネ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sample の記入例 (ウェブリンク)</t>
+    <rPh sb="8" eb="11">
+      <t>キニュウレイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>age</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4330,6 +4314,22 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="8">
@@ -4429,7 +4429,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4466,9 +4466,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -4488,8 +4496,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFBFE4FF"/>
       <color rgb="FF84919E"/>
-      <color rgb="FFBFE4FF"/>
       <color rgb="FFFFCA80"/>
       <color rgb="FFFDE9D9"/>
       <color rgb="FFDAEEF3"/>
@@ -4796,7 +4804,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -4809,7 +4817,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.5">
@@ -4819,7 +4827,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.5">
@@ -4829,12 +4837,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" s="6" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" s="14" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.5">
@@ -4842,7 +4850,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.5">
@@ -4857,7 +4865,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.5">
@@ -4865,12 +4873,12 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.5">
@@ -4921,7 +4929,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A27" s="7">
-        <v>44918</v>
+        <v>45794</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.5">
@@ -4987,7 +4995,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B37" s="7">
         <v>43227</v>
@@ -4995,7 +5003,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B38" s="7">
         <v>44103</v>
@@ -5003,7 +5011,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B39" s="7">
         <v>44622</v>
@@ -5011,7 +5019,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B40" s="7">
         <v>44678</v>
@@ -5019,7 +5027,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B41" s="7">
         <v>44918</v>
@@ -5027,10 +5035,18 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B42" s="7">
         <v>45321</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A43" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B43" s="7">
+        <v>45794</v>
       </c>
     </row>
   </sheetData>
@@ -5053,9 +5069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
@@ -5120,10 +5134,10 @@
         <v>633</v>
       </c>
       <c r="O1" s="22" t="s">
+        <v>789</v>
+      </c>
+      <c r="P1" s="22" t="s">
         <v>790</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
@@ -5152,7 +5166,7 @@
         <v>336</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>329</v>
@@ -5170,7 +5184,7 @@
         <v>607</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="P2" s="1" t="b">
         <v>1</v>
@@ -5208,7 +5222,7 @@
         <v>699</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>570</v>
@@ -5220,7 +5234,7 @@
         <v>608</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.5">
@@ -5249,7 +5263,7 @@
         <v>700</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>571</v>
@@ -5432,7 +5446,7 @@
         <v>673</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>705</v>
@@ -5461,7 +5475,7 @@
         <v>307</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>328</v>
@@ -5484,13 +5498,13 @@
         <v>650</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>308</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>706</v>
@@ -5513,7 +5527,7 @@
         <v>254</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>309</v>
@@ -5577,10 +5591,10 @@
         <v>311</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>558</v>
@@ -5626,7 +5640,7 @@
         <v>313</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>622</v>
@@ -5643,7 +5657,7 @@
         <v>314</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>623</v>
@@ -5660,7 +5674,7 @@
         <v>315</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>624</v>
@@ -5668,7 +5682,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B20" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>290</v>
@@ -5677,7 +5691,7 @@
         <v>316</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>625</v>
@@ -5685,7 +5699,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B21" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>291</v>
@@ -5694,7 +5708,7 @@
         <v>674</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="N21" s="12" t="s">
         <v>626</v>
@@ -5770,7 +5784,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B26" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>295</v>
@@ -5779,7 +5793,7 @@
         <v>320</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="N26" s="12" t="s">
         <v>631</v>
@@ -5787,7 +5801,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B27" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>296</v>
@@ -5796,7 +5810,7 @@
         <v>321</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="N27" s="12" t="s">
         <v>632</v>
@@ -5804,7 +5818,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B28" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>297</v>
@@ -5813,12 +5827,12 @@
         <v>322</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B29" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>298</v>
@@ -5832,7 +5846,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B30" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>299</v>
@@ -5846,7 +5860,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B31" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>270</v>
@@ -5860,10 +5874,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.5">
       <c r="B32" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>388</v>
@@ -5988,7 +6002,7 @@
         <v>660</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.5">
@@ -5996,7 +6010,7 @@
         <v>661</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.5">
@@ -6004,7 +6018,7 @@
         <v>662</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.5">
@@ -6033,7 +6047,7 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B51" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>716</v>
@@ -6064,17 +6078,17 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B56" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B57" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B58" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.5">
@@ -6140,12 +6154,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="18" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
@@ -6153,12 +6167,12 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="18" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
@@ -6257,7 +6271,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.5">
@@ -6408,18 +6422,18 @@
     </row>
     <row r="21" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" s="18" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
@@ -6427,7 +6441,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
@@ -6455,21 +6469,21 @@
     </row>
     <row r="30" spans="1:3" ht="52.2" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" s="20" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
@@ -6646,7 +6660,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:AD102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6657,10 +6671,13 @@
     <col min="3" max="4" width="24.88671875" style="8"/>
     <col min="5" max="6" width="24.88671875" style="1"/>
     <col min="7" max="7" width="49.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="24.88671875" style="1"/>
+    <col min="8" max="11" width="24.88671875" style="1"/>
+    <col min="12" max="12" width="74.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="32.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="24.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:30" ht="34.799999999999997" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>434</v>
       </c>
@@ -6694,11 +6711,14 @@
       <c r="K1" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L1" s="24" t="s">
+        <v>810</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A2" s="18" t="s">
         <v>7</v>
       </c>
@@ -6732,102 +6752,126 @@
       <c r="K2" s="19" t="s">
         <v>635</v>
       </c>
-      <c r="L2" s="19" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L2" s="28" t="s">
+        <v>812</v>
+      </c>
+      <c r="M2" s="28"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A3" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A4" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A5" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A6" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A7" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A8" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A9" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A10" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A12" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A13" s="22" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A15" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.5">
       <c r="A16" s="22" t="s">
         <v>29</v>
       </c>
@@ -7354,6 +7398,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="M1" r:id="rId1" location="gid=1631495971" display="Sample の記入例" xr:uid="{6A4A00BD-F6A0-4700-A260-491780AFB676}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
   <extLst>
@@ -7432,14 +7479,14 @@
       <c r="K1" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="27" t="s">
         <v>562</v>
       </c>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="18" t="s">
@@ -8686,7 +8733,7 @@
         <v>540</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>415</v>
@@ -9244,9 +9291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
@@ -9276,7 +9321,7 @@
         <v>415</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>647</v>
@@ -9300,19 +9345,19 @@
         <v>695</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>784</v>
-      </c>
       <c r="U1" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.5">
@@ -9365,19 +9410,19 @@
         <v>691</v>
       </c>
       <c r="Q2" s="23" t="s">
+        <v>784</v>
+      </c>
+      <c r="R2" s="23" t="s">
         <v>785</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="S2" s="23" t="s">
         <v>786</v>
       </c>
-      <c r="S2" s="23" t="s">
+      <c r="T2" s="23" t="s">
         <v>787</v>
       </c>
-      <c r="T2" s="23" t="s">
-        <v>788</v>
-      </c>
       <c r="U2" s="19" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.5">
@@ -9385,7 +9430,7 @@
         <v>342</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.5">
@@ -9495,9 +9540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.109375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
@@ -9586,9 +9629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
   <cols>
@@ -9599,18 +9640,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" s="18" t="s">
+        <v>740</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>741</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>